<commit_message>
Added something to prevent errors
</commit_message>
<xml_diff>
--- a/MLB/NRFI-Tracker.xlsx
+++ b/MLB/NRFI-Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbkaplinger/Desktop/Random-Projects/MLB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CA41C9-2C2A-F845-8A5C-74C814478B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0305261A-20C7-7F4B-841B-663ECE84FD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26200" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="06-30-24" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,12 @@
     <sheet name="07-04-24" sheetId="4" r:id="rId4"/>
     <sheet name="07-05-24" sheetId="5" r:id="rId5"/>
     <sheet name="07-06-24" sheetId="6" r:id="rId6"/>
+    <sheet name="07-07-24" sheetId="7" r:id="rId7"/>
+    <sheet name="07-08-24" sheetId="8" r:id="rId8"/>
+    <sheet name="07-09-24" sheetId="9" r:id="rId9"/>
+    <sheet name="07-10-24" sheetId="10" r:id="rId10"/>
+    <sheet name="07-11-24" sheetId="11" r:id="rId11"/>
+    <sheet name="07-12-24" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="84">
   <si>
     <t>Games</t>
   </si>
@@ -196,20 +202,107 @@
     <t>('CHC', 'LAA')</t>
   </si>
   <si>
+    <t>Odds</t>
+  </si>
+  <si>
+    <t>Profit/Loss</t>
+  </si>
+  <si>
+    <t>('CIN', 'COL')</t>
+  </si>
+  <si>
+    <t>('LAA', 'TEX')</t>
+  </si>
+  <si>
+    <t>('ATL', 'AZ')</t>
+  </si>
+  <si>
+    <t>('CWS', 'MIN')</t>
+  </si>
+  <si>
+    <t>('CLE', 'DET')</t>
+  </si>
+  <si>
+    <t>('KC', 'STL')</t>
+  </si>
+  <si>
+    <t>('MIL', 'PIT')</t>
+  </si>
+  <si>
+    <t>('NYY', 'TB')</t>
+  </si>
+  <si>
+    <t>('BAL', 'CHC')</t>
+  </si>
+  <si>
+    <t>('SD', 'SEA')</t>
+  </si>
+  <si>
+    <t>('HOU', 'MIA')</t>
+  </si>
+  <si>
+    <t>('BOS', 'OAK')</t>
+  </si>
+  <si>
+    <t>('LAD', 'PHI')</t>
+  </si>
+  <si>
+    <t>('SF', 'TOR')</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
-    <t>Odds</t>
-  </si>
-  <si>
-    <t>Profit/Loss</t>
+    <t>('LAA', 'SEA')</t>
+  </si>
+  <si>
+    <t>('ATL', 'SD')</t>
+  </si>
+  <si>
+    <t>('CHC', 'STL')</t>
+  </si>
+  <si>
+    <t>('COL', 'NYM')</t>
+  </si>
+  <si>
+    <t>('CLE', 'TB')</t>
+  </si>
+  <si>
+    <t>('AZ', 'TOR')</t>
+  </si>
+  <si>
+    <t>('OAK', 'PHI')</t>
+  </si>
+  <si>
+    <t>('DET', 'LAD')</t>
+  </si>
+  <si>
+    <t>('CWS', 'PIT')</t>
+  </si>
+  <si>
+    <t>('BOS', 'KC')</t>
+  </si>
+  <si>
+    <t>('HOU', 'TEX')</t>
+  </si>
+  <si>
+    <t>('MIN', 'SF')</t>
+  </si>
+  <si>
+    <t>('MIL', 'WSH')</t>
+  </si>
+  <si>
+    <t>('BAL', 'NYY')</t>
+  </si>
+  <si>
+    <t>('CIN', 'MIA')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +348,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -362,11 +491,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -386,6 +605,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,6 +1145,743 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="C2">
+        <v>-110</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>40</v>
+      </c>
+      <c r="I2">
+        <f>IF(E2=1, 1 * (100/ABS(C2)), IF(E2=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+      <c r="J2">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>-1.57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="C3">
+        <v>-140</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="C4">
+        <v>-105</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="C8">
+        <v>-140</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>IF(E8=1, 1 * (100/ABS(C8)), IF(E8=0, -1, 0))</f>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>0.58599999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C15">
+        <v>-120</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>IF(E15=1, 1 * (100/ABS(C15)), IF(E15=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>42.857142857142854</v>
+      </c>
+      <c r="J2">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>-1.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="C4">
+        <v>-150</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="C5">
+        <v>-120</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>IF(E5=1, 1 * (100/ABS(C5)), IF(E5=0, -1, 0))</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="C6">
+        <v>105</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>IF(E6=1, 1 * (100/ABS(C6)), IF(E6=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C7">
+        <v>-120</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>IF(E7=1, 1 * (100/ABS(C7)), IF(E7=0, -1, 0))</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>IF(E8=1, 1 * (100/ABS(C8)), IF(E8=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0.79</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>0.60099999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12">
+        <v>0.44400000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="C2">
+        <v>-120</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>IF(E2=1, 1 * (100/ABS(C2)), IF(E2=0, -1, 0))</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="C3">
+        <v>-135</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3">
+        <f>IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="C5">
+        <v>-130</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I16" si="0">IF(E5=1, 1 * (100/ABS(C5)), IF(E5=0, -1, 0))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>0.746</v>
+      </c>
+      <c r="C6">
+        <v>-145</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8">
+        <v>0.68700000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10">
+        <v>0.66900000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13">
+        <v>0.32300000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14">
+        <v>0.188</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="C15">
+        <v>-135</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16">
+        <v>-0.03</v>
+      </c>
+      <c r="C16" s="13">
+        <v>-135</v>
+      </c>
+      <c r="E16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H16"/>
@@ -1777,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1791,7 +2766,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1809,7 +2784,7 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
         <v>4</v>
@@ -1846,7 +2821,7 @@
       </c>
       <c r="J2">
         <f>ROUND(SUM(I2:I20), 2)</f>
-        <v>0.69</v>
+        <v>-1.31</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1859,12 +2834,12 @@
       <c r="C3">
         <v>-125</v>
       </c>
-      <c r="E3" t="s">
-        <v>52</v>
+      <c r="E3">
+        <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I15" si="0">IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
-        <v>0</v>
+        <f>IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1881,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
         <v>-1</v>
       </c>
     </row>
@@ -1910,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f>IF(E6=1, 1 * (100/ABS(C6)), IF(E6=0, -1, 0))</f>
         <v>-1</v>
       </c>
     </row>
@@ -1928,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f>IF(E7=1, 1 * (100/ABS(C7)), IF(E7=0, -1, 0))</f>
         <v>0.86956521739130432</v>
       </c>
     </row>
@@ -1946,7 +2921,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f>IF(E8=1, 1 * (100/ABS(C8)), IF(E8=0, -1, 0))</f>
         <v>0.86956521739130432</v>
       </c>
     </row>
@@ -2008,12 +2983,12 @@
       <c r="C15">
         <v>-135</v>
       </c>
-      <c r="E15" t="s">
-        <v>52</v>
+      <c r="E15">
+        <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(E15=1, 1 * (100/ABS(C15)), IF(E15=0, -1, 0))</f>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -2025,6 +3000,670 @@
       </c>
       <c r="D16" t="s">
         <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>62.5</v>
+      </c>
+      <c r="I2">
+        <f>IF(E2=1, 1 * (100/ABS(C2)), IF(E2=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+      <c r="J2" t="e">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <f>IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="e">
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="e">
+        <f>IF(E6=1, 1 * (100/ABS(C6)), IF(E6=0, -1, 0))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <f>IF(E7=1, 1 * (100/ABS(C7)), IF(E7=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8">
+        <f>IF(E8=1, 1 * (100/ABS(C8)), IF(E8=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>0.79</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>0.78</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>0.78</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>0.59299999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="C2">
+        <v>-105</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>4</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <f>IF(E2=1, 1 * (100/ABS(C2)), IF(E2=0, -1, 0))</f>
+        <v>0.95238095238095233</v>
+      </c>
+      <c r="J2">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="C3">
+        <v>-120</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>IF(E3=1, 1 * (100/ABS(C3)), IF(E3=0, -1, 0))</f>
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="C4">
+        <v>-105</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
+        <v>0.95238095238095233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C7">
+        <v>-145</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f>IF(E7=1, 1 * (100/ABS(C7)), IF(E7=0, -1, 0))</f>
+        <v>0.68965517241379315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8">
+        <v>-9.1999999999999998E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(E:E, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>COUNTA(E2:E20)</f>
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2*100</f>
+        <v>50</v>
+      </c>
+      <c r="J2">
+        <f>ROUND(SUM(I2:I20), 2)</f>
+        <v>-0.26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="C3">
+        <v>-150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="C4">
+        <v>-115</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f>IF(E4=1, 1 * (100/ABS(C4)), IF(E4=0, -1, 0))</f>
+        <v>0.86956521739130432</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="C5">
+        <v>-115</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f>IF(E5=1, 1 * (100/ABS(C5)), IF(E5=0, -1, 0))</f>
+        <v>0.86956521739130432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="C6">
+        <v>-120</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>IF(E6=1, 1 * (100/ABS(C6)), IF(E6=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7">
+        <v>0.77</v>
+      </c>
+      <c r="C7">
+        <v>-115</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>IF(E7=1, 1 * (100/ABS(C7)), IF(E7=0, -1, 0))</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8">
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>0.65100000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>0.61899999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16">
+        <v>0.255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found edge in other models
</commit_message>
<xml_diff>
--- a/MLB/NRFI-Tracker.xlsx
+++ b/MLB/NRFI-Tracker.xlsx
@@ -26,6 +26,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-23-24" sheetId="18" state="visible" r:id="rId18"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-24-24" sheetId="19" state="visible" r:id="rId19"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-25-24" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-26-24" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-27-24" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -4628,6 +4630,378 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="21" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="B1" s="21" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('CWS', 'SEA')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.732</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('CHC', 'KC')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.731</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('HOU', 'LAD')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.726</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('CLE', 'PHI')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.725</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('AZ', 'PIT')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.723</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>('LAA', 'OAK')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.719</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>('CIN', 'TB')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.718</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>('DET', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.703</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>('COL', 'SF')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.697</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>('STL', 'WSH')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.673</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>('ATL', 'NYM')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>('TEX', 'TOR')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.667</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>('MIA', 'MIL')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5639999999999999</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>('BAL', 'SD')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.556</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>('BOS', 'NYY')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.045</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="21" t="inlineStr">
+        <is>
+          <t>Games</t>
+        </is>
+      </c>
+      <c r="B1" s="21" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('CWS', 'SEA')</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('BAL', 'SD')</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.734</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('AZ', 'PIT')</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('CHC', 'KC')</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.728</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('CIN', 'TB')</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.713</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>('STL', 'WSH')</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>('HOU', 'LAD')</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.699</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>('MIA', 'MIL')</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.697</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>('BOS', 'NYY')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.6820000000000001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>('CLE', 'PHI')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.674</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>('COL', 'SF')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.575</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>('COL2', 'SF2')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.575</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>('TEX', 'TOR')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.548</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>('DET', 'MIN')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.479</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>('ATL', 'NYM')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.281</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>('LAA', 'OAK')</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Added hits allowed as a projection
</commit_message>
<xml_diff>
--- a/MLB/NRFI-Tracker.xlsx
+++ b/MLB/NRFI-Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" tabRatio="600" firstSheet="4" activeTab="18" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" tabRatio="600" firstSheet="12" activeTab="18" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="06-30-24" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,9 +25,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-22-24" sheetId="17" state="visible" r:id="rId17"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-23-24" sheetId="18" state="visible" r:id="rId18"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-24-24" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-25-24" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-26-24" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="07-27-24" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-04-24" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-06-24" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-07-24" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -157,6 +157,7 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -4525,7 +4526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4548,81 +4549,151 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>('SD', 'WSH')</t>
+          <t>('HOU', 'TB')</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.711</v>
+        <v>0.751</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>('BAL', 'MIA')</t>
+          <t>('CWS', 'MIN')</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.697</v>
+        <v>0.746</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>('LAA', 'OAK')</t>
+          <t>('PHI', 'SEA')</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.538</v>
+        <v>0.742</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>('CLE', 'DET')</t>
+          <t>('COL', 'SD')</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.514</v>
+        <v>0.737</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>('ATL', 'NYM')</t>
+          <t>('ATL', 'MIA')</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.484</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>('TB', 'TOR')</t>
+          <t>('AZ', 'PIT')</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.462</v>
+        <v>0.715</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>('LAD', 'SF')</t>
+          <t>('LAD', 'OAK')</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.456</v>
+        <v>0.714</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>('CWS', 'TEX')</t>
+          <t>('BOS', 'TEX')</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.411</v>
+        <v>0.709</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>('BAL', 'CLE')</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.709</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>('CHC', 'STL')</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.675</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>('DET', 'KC')</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>('NYY', 'TOR')</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>('CIN', 'SF')</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.407</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>('MIL', 'WSH')</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>('LAA', 'NYM')</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.117</v>
       </c>
     </row>
   </sheetData>
@@ -4659,151 +4730,151 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>('CWS', 'SEA')</t>
+          <t>('CWS', 'OAK')</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.732</v>
+        <v>0.747</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>('CHC', 'KC')</t>
+          <t>('LAD', 'PHI')</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.731</v>
+        <v>0.738</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>('HOU', 'LAD')</t>
+          <t>('SF', 'WSH')</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.726</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>('CLE', 'PHI')</t>
+          <t>('PIT', 'SD')</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.725</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>('AZ', 'PIT')</t>
+          <t>('COL', 'NYM')</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.723</v>
+        <v>0.719</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>('LAA', 'OAK')</t>
+          <t>('CHC', 'MIN')</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.719</v>
+        <v>0.711</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>('CIN', 'TB')</t>
+          <t>('HOU', 'TEX')</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.718</v>
+        <v>0.705</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>('DET', 'MIN')</t>
+          <t>('CIN', 'MIA')</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.703</v>
+        <v>0.6840000000000001</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>('COL', 'SF')</t>
+          <t>('ATL', 'MIL')</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.697</v>
+        <v>0.5610000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>('STL', 'WSH')</t>
+          <t>('AZ', 'CLE')</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.673</v>
+        <v>0.535</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>('ATL', 'NYM')</t>
+          <t>('BOS', 'KC')</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.67</v>
+        <v>0.521</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>('TEX', 'TOR')</t>
+          <t>('BAL', 'TOR')</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.667</v>
+        <v>0.478</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>('MIA', 'MIL')</t>
+          <t>('DET', 'SEA')</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.038</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>('BAL', 'SD')</t>
+          <t>('LAA', 'NYY')</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.556</v>
+        <v>-0.008</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>('BOS', 'NYY')</t>
+          <t>('STL', 'TB')</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.045</v>
+        <v>-0.126</v>
       </c>
     </row>
   </sheetData>
@@ -4817,7 +4888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4840,161 +4911,141 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>('CWS', 'SEA')</t>
+          <t>('COL', 'NYM')</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.748</v>
+        <v>0.727</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>('BAL', 'SD')</t>
+          <t>('DET', 'SEA')</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.734</v>
+        <v>0.708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>('AZ', 'PIT')</t>
+          <t>('LAD', 'PHI')</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.73</v>
+        <v>0.705</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>('CHC', 'KC')</t>
+          <t>('STL', 'TB')</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.728</v>
+        <v>0.702</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>('CIN', 'TB')</t>
+          <t>('PIT', 'SD')</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.713</v>
+        <v>0.6840000000000001</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>('STL', 'WSH')</t>
+          <t>('SF', 'WSH')</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.7</v>
+        <v>0.653</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>('HOU', 'LAD')</t>
+          <t>('CIN', 'MIA')</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.699</v>
+        <v>0.635</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>('MIA', 'MIL')</t>
+          <t>('BOS', 'KC')</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.697</v>
+        <v>0.598</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>('BOS', 'NYY')</t>
+          <t>('AZ', 'CLE')</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6820000000000001</v>
+        <v>0.5590000000000001</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>('CLE', 'PHI')</t>
+          <t>('HOU', 'TEX')</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.674</v>
+        <v>0.485</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>('COL', 'SF')</t>
+          <t>('CHC', 'MIN')</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.575</v>
+        <v>0.463</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>('COL2', 'SF2')</t>
+          <t>('BAL', 'TOR')</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.575</v>
+        <v>0.319</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>('TEX', 'TOR')</t>
+          <t>('ATL', 'MIL')</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.548</v>
+        <v>0.163</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>('DET', 'MIN')</t>
+          <t>('CWS', 'OAK')</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.479</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>('ATL', 'NYM')</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.281</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>('LAA', 'OAK')</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>0.245</v>
+        <v>-0.08699999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>